<commit_message>
modified tendon length values
</commit_message>
<xml_diff>
--- a/muscle_length_determination/ligament_and_muscle_lengths.xlsx
+++ b/muscle_length_determination/ligament_and_muscle_lengths.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Tokyo Tech\Project\Dog Robot\Hoshiramu_robot\muscle_length_determination\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{9279C57E-5F5A-4B6C-9BAB-94F8C0316C59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{8882341B-4697-4183-8A24-D15EF06E3577}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{9279C57E-5F5A-4B6C-9BAB-94F8C0316C59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{10BFD0DB-80F1-4B37-AABA-A359C05374D7}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="2" xr2:uid="{26156378-0049-4A8B-8CB0-3F3BBDC12CF9}"/>
   </bookViews>
@@ -943,7 +943,7 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -973,7 +973,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B2">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -1007,7 +1007,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>8</v>
@@ -1087,7 +1087,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <v>8</v>
@@ -1112,7 +1112,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C14">
         <v>20</v>
@@ -1149,7 +1149,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B17">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C17">
         <v>20</v>
@@ -1186,7 +1186,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B20">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C20">
         <v>20</v>
@@ -1217,7 +1217,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B23">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C23">
         <v>20</v>
@@ -1251,7 +1251,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B26">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C26">
         <v>22</v>
@@ -1285,7 +1285,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B29">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C29">
         <v>70</v>

</xml_diff>

<commit_message>
modified matlab code & added new add-on components
</commit_message>
<xml_diff>
--- a/muscle_length_determination/ligament_and_muscle_lengths.xlsx
+++ b/muscle_length_determination/ligament_and_muscle_lengths.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Tokyo Tech\Project\Dog Robot\Hoshiramu_robot\muscle_length_determination\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{9279C57E-5F5A-4B6C-9BAB-94F8C0316C59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{10BFD0DB-80F1-4B37-AABA-A359C05374D7}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{9279C57E-5F5A-4B6C-9BAB-94F8C0316C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10BFD0DB-80F1-4B37-AABA-A359C05374D7}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="2" xr2:uid="{26156378-0049-4A8B-8CB0-3F3BBDC12CF9}"/>
   </bookViews>
@@ -17,10 +17,21 @@
     <sheet name="Muscles(L)" sheetId="2" r:id="rId2"/>
     <sheet name="Tendons(L)" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -206,9 +217,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -246,7 +257,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -352,7 +363,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -494,7 +505,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -508,9 +519,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,7 +544,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>23</v>
       </c>
@@ -553,7 +564,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -576,7 +587,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>29</v>
       </c>
@@ -596,7 +607,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -619,7 +630,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>28</v>
       </c>
@@ -639,7 +650,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -656,7 +667,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>20</v>
       </c>
@@ -670,7 +681,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -687,7 +698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>13</v>
       </c>
@@ -716,9 +727,9 @@
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -732,12 +743,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -754,12 +765,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -782,12 +793,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>257</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -801,12 +812,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>252</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -817,12 +828,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>218</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -839,12 +850,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -861,12 +872,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>165</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -880,12 +891,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>165</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -902,12 +913,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>219</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -921,12 +932,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>226</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -943,12 +954,12 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -971,7 +982,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>7</v>
       </c>
@@ -979,7 +990,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1005,7 +1016,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>7</v>
       </c>
@@ -1013,7 +1024,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1054,7 +1065,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5</v>
       </c>
@@ -1062,7 +1073,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1085,7 +1096,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>4</v>
       </c>
@@ -1093,7 +1104,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1110,7 +1121,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>7</v>
       </c>
@@ -1118,7 +1129,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1147,7 +1158,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>7</v>
       </c>
@@ -1155,7 +1166,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1184,7 +1195,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>7</v>
       </c>
@@ -1192,7 +1203,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1215,7 +1226,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>7</v>
       </c>
@@ -1223,7 +1234,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -1249,7 +1260,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>5</v>
       </c>
@@ -1260,7 +1271,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1283,7 +1294,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
added muscle lengths for other reference marks
</commit_message>
<xml_diff>
--- a/muscle_length_determination/ligament_and_muscle_lengths.xlsx
+++ b/muscle_length_determination/ligament_and_muscle_lengths.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Tokyo Tech\Project\Dog Robot\Hoshiramu_robot\muscle_length_determination\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{9279C57E-5F5A-4B6C-9BAB-94F8C0316C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10BFD0DB-80F1-4B37-AABA-A359C05374D7}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{9279C57E-5F5A-4B6C-9BAB-94F8C0316C59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA0C4B86-F625-4300-80BF-84AEF368B8C5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="2" xr2:uid="{26156378-0049-4A8B-8CB0-3F3BBDC12CF9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1" xr2:uid="{26156378-0049-4A8B-8CB0-3F3BBDC12CF9}"/>
   </bookViews>
   <sheets>
     <sheet name="Ligaments" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Tendons(L)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,10 +28,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -217,9 +218,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -257,7 +258,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -363,7 +364,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -505,7 +506,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -519,9 +520,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -544,7 +545,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>23</v>
       </c>
@@ -564,7 +565,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -587,7 +588,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>29</v>
       </c>
@@ -607,7 +608,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -630,7 +631,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>28</v>
       </c>
@@ -650,7 +651,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -667,7 +668,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>20</v>
       </c>
@@ -681,7 +682,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -698,7 +699,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>13</v>
       </c>
@@ -723,13 +724,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC300D97-1AF3-46AE-9AA4-448FF1ABE50C}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -743,12 +744,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="C2">
+        <v>140</v>
+      </c>
+      <c r="D2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -765,12 +772,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -793,12 +800,27 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8">
+        <v>255</v>
+      </c>
+      <c r="C8">
+        <v>260</v>
+      </c>
+      <c r="D8">
+        <v>263</v>
+      </c>
+      <c r="E8">
+        <v>258</v>
+      </c>
+      <c r="F8">
         <v>257</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -812,12 +834,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="C11">
+        <v>255</v>
+      </c>
+      <c r="D11">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -828,12 +856,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>218</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -850,12 +881,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>173</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>153</v>
+      </c>
+      <c r="D17">
+        <v>152</v>
+      </c>
+      <c r="E17">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -872,12 +912,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>165</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -891,12 +931,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>165</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -913,12 +953,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B26">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+      <c r="C26">
+        <v>220</v>
+      </c>
+      <c r="D26">
+        <v>214</v>
+      </c>
+      <c r="E26">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -932,12 +981,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>226</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>227</v>
+      </c>
+      <c r="D29">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -953,13 +1008,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB99F533-89CE-4002-A23E-0EB847934D80}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -982,7 +1037,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>7</v>
       </c>
@@ -990,7 +1045,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1016,7 +1071,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>7</v>
       </c>
@@ -1024,7 +1079,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1065,7 +1120,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>5</v>
       </c>
@@ -1073,7 +1128,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1096,7 +1151,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>4</v>
       </c>
@@ -1104,7 +1159,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1121,7 +1176,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>7</v>
       </c>
@@ -1129,7 +1184,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1158,7 +1213,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>7</v>
       </c>
@@ -1166,7 +1221,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1195,7 +1250,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>7</v>
       </c>
@@ -1203,7 +1258,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1226,7 +1281,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>7</v>
       </c>
@@ -1234,7 +1289,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -1260,7 +1315,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>5</v>
       </c>
@@ -1271,7 +1326,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1294,7 +1349,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>27</v>
       </c>

</xml_diff>